<commit_message>
//leaves code up to date till 6/28/2019
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project_sikhar\leave\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F83A383-D5A5-435D-A86D-477F85982314}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B24B3B-1A94-4132-B643-B7A74BBFBE35}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4848" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1"/>
@@ -66,7 +66,7 @@
     <t>wild1</t>
   </si>
   <si>
-    <t>16</t>
+    <t>26,28,29,30,31,36</t>
   </si>
   <si>
     <t>Automation1</t>
@@ -444,7 +444,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="8.5546875"/>
+    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.21875"/>
     <col min="4" max="4" width="20"/>
     <col min="5" max="5" width="9.77734375"/>

</xml_diff>

<commit_message>
Leave Balance Code- Custom leave cycle
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{570666F6-44D3-43A2-B6F9-FDFB44D8FA52}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FFBE3E-C832-48DE-A306-FB8E0780A45F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,7 +69,7 @@
     <t>Automation1</t>
   </si>
   <si>
-    <t>34</t>
+    <t>38</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
leave balance 1.4L scenaioes updated code
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80FFBE3E-C832-48DE-A306-FB8E0780A45F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE9798F-E4F7-4380-88C0-7FDDF5B5B448}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,10 +66,10 @@
     <t>wild1</t>
   </si>
   <si>
-    <t>Automation1</t>
-  </si>
-  <si>
-    <t>38</t>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Automation3</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -477,13 +477,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
leave balance 1.4L scenaioes updated code _v1
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EE9798F-E4F7-4380-88C0-7FDDF5B5B448}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736B2530-F644-4915-A061-E2EB672DA2B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
leave balance 1.4L scenaioes updated code _v2
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{736B2530-F644-4915-A061-E2EB672DA2B3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6CE8E84-9840-4297-B0A3-A08D506775A1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working days november  run 2 without probation,without end of year
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9825F78-EC31-493B-B630-5589CBFD26F1}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770E2C58-43F4-4D32-A8C7-2F95F9041DA5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3864" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -66,7 +66,7 @@
     <t>wild1</t>
   </si>
   <si>
-    <t>Automation2</t>
+    <t>Automation3</t>
   </si>
   <si>
     <t>43</t>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
leave balance run 2
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D86B2A9-6106-40A4-8CA9-A5BC2B107F0D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA489D74-0591-450C-84C3-B6723EB71762}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4212" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -66,10 +66,10 @@
     <t>wild1</t>
   </si>
   <si>
-    <t>43</t>
-  </si>
-  <si>
-    <t>Automation2</t>
+    <t>42</t>
+  </si>
+  <si>
+    <t>Automation3</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
working days - october
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A233D64-F363-4264-976D-08CD785C106E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B395D-A6EC-46A5-95EE-C37BC84988F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4212" yWindow="3396" windowWidth="17280" windowHeight="8964" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -66,13 +66,13 @@
     <t>wild1</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Automation3</t>
-  </si>
-  <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>Automation2</t>
+  </si>
+  <si>
+    <t>43</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
@@ -500,7 +500,7 @@
         <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
working days - september  run
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F49B395D-A6EC-46A5-95EE-C37BC84988F0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F81A5E42-A3F5-4144-8861-C9FD40A70F0C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>1</t>
   </si>
   <si>
+    <t>43</t>
+  </si>
+  <si>
     <t>Automation2</t>
-  </si>
-  <si>
-    <t>43</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -480,13 +480,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
leave balance 1-10 policies
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD04CDD-4BF0-417D-8FD1-8CBE7CBD8CF8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7F7AB1D-24C8-459F-84B1-3A6664E0EAC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Automation3</t>
-  </si>
-  <si>
-    <t>44</t>
+    <t>Automation2</t>
+  </si>
+  <si>
+    <t>42</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
deactivation - november cycle
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B1D9F8F-1AF4-4A73-B3B9-1632B864BDC6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8BC74C1-C031-4ECD-AD6C-17CB635E4F4D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
-    <t>Automation2</t>
+    <t>40</t>
+  </si>
+  <si>
+    <t>Automation1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
//Leave Application - Hourly
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Automation_Project\leave\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\OneDrive\Desktop\core-automation\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3BBB827-BB90-4FA2-94B3-6B35C5EC566D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{F3BBB827-BB90-4FA2-94B3-6B35C5EC566D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{4CCA1139-338F-4761-B5F9-9C0014F97207}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Automation2</t>
-  </si>
-  <si>
-    <t>45</t>
+    <t>48</t>
+  </si>
+  <si>
+    <t>Automation3</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -486,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
//leaves - add  Readme.txt
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AE35EE-0F73-491A-B537-E009F987E2B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77A5557F-11F8-4ECD-B69F-A268B96ACA3C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>Automation2</t>
   </si>
   <si>
-    <t>40</t>
+    <t>44</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
//leave Balnce - cases split up
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CA8DAA-670B-4BFF-8D53-E60BE6BF2145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC97100-29C2-4AAE-B913-4A74E97740B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Automation3</t>
-  </si>
-  <si>
-    <t>34</t>
+    <t>Automation2</t>
+  </si>
+  <si>
+    <t>42,43,44,45</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Revert "Merge branch 'origin/yetendra' into 'master'"
This reverts merge request !14
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EC97100-29C2-4AAE-B913-4A74E97740B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CA8DAA-670B-4BFF-8D53-E60BE6BF2145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Automation2</t>
-  </si>
-  <si>
-    <t>42,43,44,45</t>
+    <t>Automation3</t>
+  </si>
+  <si>
+    <t>34</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
//leaves - BAL case split
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7CA8DAA-670B-4BFF-8D53-E60BE6BF2145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B1F2482-1853-427F-8E9B-91FA59B8CC65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>Automation3</t>
-  </si>
-  <si>
-    <t>34</t>
+    <t>42-45</t>
+  </si>
+  <si>
+    <t>Automation1</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -486,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
carry forward failure fixes
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF573633-161B-414F-B558-AF45E14E6611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D400B5A-E5C8-4B39-B989-BB7DF1FDC263}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>42</t>
-  </si>
-  <si>
     <t>Automation2</t>
+  </si>
+  <si>
+    <t>40</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -486,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
carry forward percentage run
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE315118-35D3-4995-8F9F-70C82A17E5BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A77D56B-5023-4394-858A-105DDDCBE030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>54</t>
   </si>
   <si>
-    <t>Automation2</t>
+    <t>Automation1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
carry forward hourly run
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A77D56B-5023-4394-858A-105DDDCBE030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD12B2C-F5A9-4657-8C52-BCC8E524C6E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>54</t>
-  </si>
-  <si>
-    <t>Automation1</t>
+    <t>Automation2</t>
+  </si>
+  <si>
+    <t>55</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -486,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Leave Balance - Hourly Run
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A5EC570-5367-44E5-8472-ECD0CF91D49D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21543E8E-C1C1-48C0-B7A6-2D0034619B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>55</t>
   </si>
   <si>
-    <t>Automation3</t>
+    <t>Automation4</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
updated leave module as on 3/16/2020
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\IdeaProjects\Master\Automation_Project\leave\src\main\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21543E8E-C1C1-48C0-B7A6-2D0034619B04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5F1E510-79FD-429C-A0C3-9F89FFC22F49}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="468" yWindow="1116" windowWidth="22572" windowHeight="11844" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,10 @@
     <t>1</t>
   </si>
   <si>
-    <t>55</t>
-  </si>
-  <si>
-    <t>Automation4</t>
+    <t>51</t>
+  </si>
+  <si>
+    <t>Automation5</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CF WITH wd run2
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\yeten\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF54DE46-DA24-435D-BB8F-C87A56401A23}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7B5D28A-4449-4B6E-99AD-2E40E34B5A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="22572" windowHeight="11844" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="468" yWindow="1116" windowWidth="22572" windowHeight="11844" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -63,10 +63,10 @@
     <t>Sanity.xlsx</t>
   </si>
   <si>
-    <t>45</t>
-  </si>
-  <si>
     <t>Automation5</t>
+  </si>
+  <si>
+    <t>69</t>
   </si>
 </sst>
 </file>
@@ -466,13 +466,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
1.changed the folder structure  2.added cases for ma missed scenrioes
</commit_message>
<xml_diff>
--- a/leave/src/main/resources/Config.xlsx
+++ b/leave/src/main/resources/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sande\Desktop\yeten\Automation_Project\leave\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D246B8A9-60FC-48FD-9A48-8B325EF46866}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EF0943-8284-42B1-AB26-D7F9A2B0112D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="468" yWindow="768" windowWidth="22572" windowHeight="11844" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="2" r:id="rId1"/>
@@ -60,13 +60,13 @@
     <t>DEBUG</t>
   </si>
   <si>
-    <t>Automation3</t>
-  </si>
-  <si>
     <t>all</t>
   </si>
   <si>
-    <t>WeeklySanity.xlsx</t>
+    <t>Automation5</t>
+  </si>
+  <si>
+    <t>Sanity.xlsx</t>
   </si>
 </sst>
 </file>
@@ -436,10 +436,13 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="13" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -466,13 +469,13 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>